<commit_message>
update monthly and yearly outcome_ath dictionaries
</commit_message>
<xml_diff>
--- a/dictionaries/outcome_ath/1_0/1_0_monthly_rep.xlsx
+++ b/dictionaries/outcome_ath/1_0/1_0_monthly_rep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\back\ATHLETE\HARMO\20220613_dicts\extender_outcomes_ath\respuestas16dic2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{ADBFBF70-69A4-4A0C-86C9-C810047AE939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE13494C-9C8B-471A-8123-CF87281F7409}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{ADBFBF70-69A4-4A0C-86C9-C810047AE939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93627684-7557-4909-90B7-64BBD471F6EC}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="-6600" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
     <t>numeric</t>
   </si>
   <si>
-    <t>Unique identifer for the row in Opal</t>
+    <t>Unique identifier for the row in Opal</t>
   </si>
   <si>
     <t>child_id</t>
@@ -66,7 +66,7 @@
     <t>text</t>
   </si>
   <si>
-    <t>Unique identifer for the child</t>
+    <t>Unique identifier for the child</t>
   </si>
   <si>
     <t>age_years</t>
@@ -639,7 +639,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>

</xml_diff>